<commit_message>
Moved the old models into a folder, and created output excel files for some runs
</commit_message>
<xml_diff>
--- a/CFI-Levelized-Cost-of-Energy.xlsx
+++ b/CFI-Levelized-Cost-of-Energy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spide\Documents\TU Delft\Thesis Project\MSc Thesis - Piotr K\PiotrThesis\PiotrThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E90181E7-4E7C-4ED1-9A0A-C506088E143D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8868FC6-0DD5-41C0-B9C9-98367C6D5C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6832477F-F6C6-4EB0-86B1-4E06BC66BACA}"/>
   </bookViews>
@@ -172,7 +172,7 @@
     <numFmt numFmtId="175" formatCode="#,##0;\(#,##0\);\-"/>
     <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="177" formatCode="#,##0&quot;kWh&quot;;\(#,##0\)&quot;kWh&quot;;\-"/>
-    <numFmt numFmtId="184" formatCode="&quot;$&quot;#,##0.0000000&quot;/kWh&quot;;\(&quot;$&quot;#,##0.0000000\)&quot;/kWh&quot;;\-"/>
+    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.0000000&quot;/kWh&quot;;\(&quot;$&quot;#,##0.0000000\)&quot;/kWh&quot;;\-"/>
   </numFmts>
   <fonts count="35">
     <font>
@@ -756,7 +756,7 @@
     <xf numFmtId="171" fontId="34" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="184" fontId="27" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="178" fontId="27" fillId="0" borderId="11" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1596,7 +1596,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3686,20 +3686,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b2efed34-04dd-4047-8bed-7b982d739149" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b2efed34-04dd-4047-8bed-7b982d739149" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3722,14 +3722,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DB49FE-32A7-4D53-971D-F2C4DE6C011E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{921AA4FE-CA4F-40B5-8F66-C983756B6902}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="6e38cd29-cea5-4f67-ad1f-a4b1dbbd2880"/>
@@ -3744,4 +3736,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DB49FE-32A7-4D53-971D-F2C4DE6C011E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>